<commit_message>
- Amélioré le traitement des villes étrangères lors de l'importation des données. Pour cela,   j'ai rajouté une colonne Pays dans les fichiers paroissiaux pour déterminer de quel pays   est l'adresse. Dans le cas où aucun pays n'est spécifié, on assume que c'est la Suisse. Cela   permet ensuite de se baser là-dessus plutôt que d'essayer de deviner selon le numéro postal   de quel pays vient la ville.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20341 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Région 9/9040/person1.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Région 9/9040/person1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7754" uniqueCount="1996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7755" uniqueCount="1997">
   <si>
     <t>_id</t>
   </si>
@@ -6002,6 +6002,9 @@
   </si>
   <si>
     <t>12/11/1971</t>
+  </si>
+  <si>
+    <t>Pays</t>
   </si>
 </sst>
 </file>
@@ -6045,7 +6048,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -6109,6 +6112,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6411,15 +6417,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA601"/>
+  <dimension ref="A1:BB601"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BB1" sqref="BB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6579,8 +6585,11 @@
       <c r="BA1" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BB1" s="22" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>192956</v>
       </c>
@@ -6633,7 +6642,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>192957</v>
       </c>
@@ -6683,7 +6692,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>192958</v>
       </c>
@@ -6736,7 +6745,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>192959</v>
       </c>
@@ -6789,7 +6798,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>192960</v>
       </c>
@@ -6842,7 +6851,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>192961</v>
       </c>
@@ -6892,7 +6901,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>192962</v>
       </c>
@@ -6942,7 +6951,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>192963</v>
       </c>
@@ -6992,7 +7001,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>192964</v>
       </c>
@@ -7048,7 +7057,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>192965</v>
       </c>
@@ -7101,7 +7110,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>192966</v>
       </c>
@@ -7154,7 +7163,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>192967</v>
       </c>
@@ -7207,7 +7216,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>192968</v>
       </c>
@@ -7260,7 +7269,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>192969</v>
       </c>
@@ -7313,7 +7322,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>192970</v>
       </c>

</xml_diff>